<commit_message>
modified with day 4
</commit_message>
<xml_diff>
--- a/51daysofcode/records.xlsx
+++ b/51daysofcode/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Desktop\Code It\competitive platform\51daysofcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82AFB99E-FBF6-4420-B56F-539E03F9E3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD2D9B-D2C9-44F5-8E45-D5C5B07A7B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1DA2034A-82B9-4E8D-B441-FDD9FDD9DAB6}"/>
   </bookViews>
@@ -410,12 +410,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="87.33203125" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>